<commit_message>
New mealgenerator with dataframe + some short update
</commit_message>
<xml_diff>
--- a/TableS1_augmented_with_FAO_data.xlsx
+++ b/TableS1_augmented_with_FAO_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cknibbe/Documents/teach-INSA/2020-2021/modules/algoprog/poore2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanis.000\Desktop\0cours\3a-s2\info algo\environment_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1713A1-B0D8-8346-8237-4A6A6A2B9B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F52A75-840E-48B3-9AF6-7039A3DAE737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3560" windowWidth="27640" windowHeight="16940" xr2:uid="{EA922DF9-20B0-DA49-97C5-31EEC4E82887}"/>
+    <workbookView xWindow="1890" yWindow="1350" windowWidth="25665" windowHeight="14985" xr2:uid="{EA922DF9-20B0-DA49-97C5-31EEC4E82887}"/>
   </bookViews>
   <sheets>
     <sheet name="FAOdata" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="92">
   <si>
     <t xml:space="preserve">1000 kcal energy </t>
   </si>
@@ -302,6 +312,9 @@
   </si>
   <si>
     <t>Fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 kg of fat and bone-free meat and edible offal </t>
   </si>
 </sst>
 </file>
@@ -13900,20 +13913,20 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="34">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="31.5">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -14871,8 +14884,14 @@
       <c r="A36" t="s">
         <v>40</v>
       </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
       <c r="C36" t="s">
         <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>91</v>
       </c>
       <c r="E36">
         <v>1500</v>
@@ -15231,16 +15250,16 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="34">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>

</xml_diff>